<commit_message>
Update servo board BOM
Generated by bomtool - see recent commit history on that repo.
</commit_message>
<xml_diff>
--- a/quote-pack/servo/servo-bom.xlsx
+++ b/quote-pack/servo/servo-bom.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="369">
   <si>
     <t>Part</t>
   </si>
@@ -163,12 +163,18 @@
     <t>sr-c-1u-0402-10v</t>
   </si>
   <si>
-    <t>SMD Capacitor, 1uF, 10%, 10V (16V is suitable), 0402</t>
+    <t>1u capacitor 0402 10V X5R</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
+    <t>1458896</t>
+  </si>
+  <si>
+    <t>https://uk.farnell.com/-/-/-/dp/1458896</t>
+  </si>
+  <si>
     <t>C20</t>
   </si>
   <si>
@@ -304,16 +310,10 @@
     <t>Pluggable terminal block 2way 7.5mm pitch male horiz</t>
   </si>
   <si>
-    <t>rapid</t>
-  </si>
-  <si>
-    <t>21-2448</t>
-  </si>
-  <si>
-    <t>https://www.rapidonline.com/Catalogue/Search?Query=21-2448</t>
-  </si>
-  <si>
-    <t>low stock (want 172, while only 227 are available)</t>
+    <t>3882391</t>
+  </si>
+  <si>
+    <t>https://uk.farnell.com/-/-/-/dp/3882391</t>
   </si>
   <si>
     <t>J5</t>
@@ -412,7 +412,7 @@
     <t>camcon_38_4</t>
   </si>
   <si>
-    <t>CTB93HE/4 – Pluggable terminal block 4way 3.81mm pitch male horiz</t>
+    <t>Pluggable terminal block 4way 3.81mm pitch male horiz</t>
   </si>
   <si>
     <t>1717073</t>
@@ -499,10 +499,10 @@
     <t>zener diode 5.1V 150mW</t>
   </si>
   <si>
-    <t>755-EDZTE615.1B</t>
-  </si>
-  <si>
-    <t>https://www.mouser.co.uk/ProductDetail/ROHM-Semiconductor/EDZTE6151B?qs=4kLU8WoGk0uAJO8EOvJm8g%3D%3D</t>
+    <t>2536475</t>
+  </si>
+  <si>
+    <t>https://uk.farnell.com/-/-/-/dp/2536475</t>
   </si>
   <si>
     <t>D15, D13, D18, D3, D14, D17, D12</t>
@@ -673,10 +673,10 @@
     <t>INA219AIDCNR I2C current sense amp</t>
   </si>
   <si>
-    <t>2295989</t>
-  </si>
-  <si>
-    <t>https://uk.farnell.com/-/-/-/dp/2295989</t>
+    <t>3118164</t>
+  </si>
+  <si>
+    <t>https://uk.farnell.com/-/-/-/dp/3118164</t>
   </si>
   <si>
     <t>U1</t>
@@ -754,10 +754,10 @@
     <t>3V-14.4V input 0.6V-5.5V output 12A non-isolated DC-DC module</t>
   </si>
   <si>
-    <t>894-PVX012A0X3-SRZ</t>
-  </si>
-  <si>
-    <t>https://www.mouser.co.uk/ProductDetail/ABB-Embedded-Power/PVX012A0X3-SRZ?qs=FZWyocRRknmGQ1lZtu1e%2FQ%3D%3D</t>
+    <t>2076909</t>
+  </si>
+  <si>
+    <t>https://uk.farnell.com/-/-/-/dp/2076909</t>
   </si>
   <si>
     <t>U8</t>
@@ -796,10 +796,10 @@
     <t>USB EMI/ESD protection and termination</t>
   </si>
   <si>
-    <t>863-STF202-22T1G</t>
-  </si>
-  <si>
-    <t>https://www.mouser.co.uk/ProductDetail/ON-Semiconductor/STF202-22T1G?qs=xZq1yRCsb1dM1UQ1NtNRtw%3D%3D</t>
+    <t>1651958</t>
+  </si>
+  <si>
+    <t>https://uk.farnell.com/-/-/-/dp/1651958</t>
   </si>
   <si>
     <t>U2</t>
@@ -1489,10 +1489,14 @@
         <v>26</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
@@ -1510,19 +1514,19 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
@@ -1556,19 +1560,19 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
@@ -1584,10 +1588,10 @@
         <v>44</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
@@ -1606,23 +1610,23 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>25</v>
@@ -1634,10 +1638,10 @@
         <v>44</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
@@ -1656,23 +1660,23 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>25</v>
@@ -1684,10 +1688,10 @@
         <v>44</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
@@ -1706,19 +1710,19 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
@@ -1734,10 +1738,10 @@
         <v>44</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
@@ -1756,19 +1760,19 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
@@ -1781,13 +1785,13 @@
         <v>26</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
@@ -1806,19 +1810,19 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
@@ -1831,17 +1835,15 @@
         <v>26</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="M13" s="2" t="s">
         <v>100</v>
       </c>
+      <c r="M13" s="2"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
@@ -2224,7 +2226,7 @@
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>25</v>
@@ -2283,7 +2285,7 @@
         <v>26</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>162</v>
@@ -2424,7 +2426,7 @@
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>25</v>
@@ -2524,7 +2526,7 @@
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>25</v>
@@ -2667,7 +2669,7 @@
         <v>211</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>212</v>
@@ -2933,7 +2935,7 @@
         <v>26</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="K35" s="2" t="s">
         <v>247</v>
@@ -2983,7 +2985,7 @@
         <v>26</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="K36" s="2" t="s">
         <v>254</v>
@@ -3033,7 +3035,7 @@
         <v>26</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="K37" s="2" t="s">
         <v>261</v>
@@ -3274,7 +3276,7 @@
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>25</v>
@@ -3324,7 +3326,7 @@
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>25</v>
@@ -3689,7 +3691,7 @@
         <v>334</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>335</v>
@@ -3746,7 +3748,7 @@
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>25</v>
@@ -30409,48 +30411,49 @@
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="L5"/>
-    <hyperlink r:id="rId2" ref="L8"/>
-    <hyperlink r:id="rId3" ref="L9"/>
-    <hyperlink r:id="rId4" ref="L10"/>
-    <hyperlink r:id="rId5" ref="L11"/>
-    <hyperlink r:id="rId6" ref="L12"/>
-    <hyperlink r:id="rId7" ref="L13"/>
-    <hyperlink r:id="rId8" ref="L14"/>
-    <hyperlink r:id="rId9" ref="L15"/>
-    <hyperlink r:id="rId10" ref="L16"/>
-    <hyperlink r:id="rId11" ref="L17"/>
-    <hyperlink r:id="rId12" ref="L18"/>
-    <hyperlink r:id="rId13" ref="L19"/>
-    <hyperlink r:id="rId14" ref="L20"/>
-    <hyperlink r:id="rId15" ref="L21"/>
-    <hyperlink r:id="rId16" ref="L22"/>
-    <hyperlink r:id="rId17" ref="L23"/>
-    <hyperlink r:id="rId18" ref="L24"/>
-    <hyperlink r:id="rId19" ref="L25"/>
-    <hyperlink r:id="rId20" ref="L26"/>
-    <hyperlink r:id="rId21" ref="L27"/>
-    <hyperlink r:id="rId22" ref="L28"/>
-    <hyperlink r:id="rId23" ref="L29"/>
-    <hyperlink r:id="rId24" ref="L30"/>
-    <hyperlink r:id="rId25" ref="L31"/>
-    <hyperlink r:id="rId26" ref="L32"/>
-    <hyperlink r:id="rId27" ref="L33"/>
-    <hyperlink r:id="rId28" ref="L34"/>
-    <hyperlink r:id="rId29" ref="L35"/>
-    <hyperlink r:id="rId30" ref="L36"/>
-    <hyperlink r:id="rId31" ref="L37"/>
-    <hyperlink r:id="rId32" ref="L38"/>
-    <hyperlink r:id="rId33" ref="L39"/>
-    <hyperlink r:id="rId34" ref="L40"/>
-    <hyperlink r:id="rId35" ref="L41"/>
-    <hyperlink r:id="rId36" ref="L42"/>
-    <hyperlink r:id="rId37" ref="L48"/>
-    <hyperlink r:id="rId38" ref="L51"/>
-    <hyperlink r:id="rId39" ref="L53"/>
-    <hyperlink r:id="rId40" ref="L54"/>
-    <hyperlink r:id="rId41" ref="L55"/>
-    <hyperlink r:id="rId42" ref="L56"/>
+    <hyperlink r:id="rId2" ref="L6"/>
+    <hyperlink r:id="rId3" ref="L8"/>
+    <hyperlink r:id="rId4" ref="L9"/>
+    <hyperlink r:id="rId5" ref="L10"/>
+    <hyperlink r:id="rId6" ref="L11"/>
+    <hyperlink r:id="rId7" ref="L12"/>
+    <hyperlink r:id="rId8" ref="L13"/>
+    <hyperlink r:id="rId9" ref="L14"/>
+    <hyperlink r:id="rId10" ref="L15"/>
+    <hyperlink r:id="rId11" ref="L16"/>
+    <hyperlink r:id="rId12" ref="L17"/>
+    <hyperlink r:id="rId13" ref="L18"/>
+    <hyperlink r:id="rId14" ref="L19"/>
+    <hyperlink r:id="rId15" ref="L20"/>
+    <hyperlink r:id="rId16" ref="L21"/>
+    <hyperlink r:id="rId17" ref="L22"/>
+    <hyperlink r:id="rId18" ref="L23"/>
+    <hyperlink r:id="rId19" ref="L24"/>
+    <hyperlink r:id="rId20" ref="L25"/>
+    <hyperlink r:id="rId21" ref="L26"/>
+    <hyperlink r:id="rId22" ref="L27"/>
+    <hyperlink r:id="rId23" ref="L28"/>
+    <hyperlink r:id="rId24" ref="L29"/>
+    <hyperlink r:id="rId25" ref="L30"/>
+    <hyperlink r:id="rId26" ref="L31"/>
+    <hyperlink r:id="rId27" ref="L32"/>
+    <hyperlink r:id="rId28" ref="L33"/>
+    <hyperlink r:id="rId29" ref="L34"/>
+    <hyperlink r:id="rId30" ref="L35"/>
+    <hyperlink r:id="rId31" ref="L36"/>
+    <hyperlink r:id="rId32" ref="L37"/>
+    <hyperlink r:id="rId33" ref="L38"/>
+    <hyperlink r:id="rId34" ref="L39"/>
+    <hyperlink r:id="rId35" ref="L40"/>
+    <hyperlink r:id="rId36" ref="L41"/>
+    <hyperlink r:id="rId37" ref="L42"/>
+    <hyperlink r:id="rId38" ref="L48"/>
+    <hyperlink r:id="rId39" ref="L51"/>
+    <hyperlink r:id="rId40" ref="L53"/>
+    <hyperlink r:id="rId41" ref="L54"/>
+    <hyperlink r:id="rId42" ref="L55"/>
+    <hyperlink r:id="rId43" ref="L56"/>
   </hyperlinks>
-  <drawing r:id="rId43"/>
+  <drawing r:id="rId44"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add mouser link for U2 since Farnell and Mouser both have limited stock
</commit_message>
<xml_diff>
--- a/quote-pack/servo/servo-bom.xlsx
+++ b/quote-pack/servo/servo-bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="371">
   <si>
     <t xml:space="preserve">Part</t>
   </si>
@@ -830,6 +830,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://uk.farnell.com/-/-/-/dp/2333160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">511-STM32F103C6U6A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.co.uk/ProductDetail/STMicroelectronics/STM32F103C6U6A?qs=%2Fha2pyFaduhWlUF2EGqvyLw8AQJjPxdFr9%2FgAGUmVdrlf0EAElETsQ%3D%3D</t>
   </si>
   <si>
     <t xml:space="preserve">DS11, DS6, DS12, DS7, DS2, DS14, DS13, DS9, DS3, DS8, DS4, DS5</t>
@@ -1217,7 +1223,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1238,6 +1244,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1255,10 +1265,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z1048576"/>
+  <dimension ref="A1:Z57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L37" activeCellId="0" sqref="L37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K40" activeCellId="0" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1266,18 +1276,18 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="23.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="114.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="41.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="9.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="17" style="0" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="14.43"/>
@@ -3183,25 +3193,25 @@
       <c r="Y38" s="3"/>
       <c r="Z38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
-        <v>275</v>
+        <v>38</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>25</v>
@@ -3210,13 +3220,13 @@
         <v>26</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
@@ -3233,25 +3243,25 @@
       <c r="Y39" s="3"/>
       <c r="Z39" s="3"/>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
-        <v>33</v>
+        <v>277</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>25</v>
@@ -3263,10 +3273,10 @@
         <v>44</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="L40" s="4" t="s">
-        <v>283</v>
+        <v>278</v>
+      </c>
+      <c r="L40" s="5" t="s">
+        <v>279</v>
       </c>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
@@ -3285,23 +3295,23 @@
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>25</v>
@@ -3313,10 +3323,10 @@
         <v>44</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
@@ -3335,23 +3345,23 @@
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>153</v>
+        <v>289</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>25</v>
@@ -3363,10 +3373,10 @@
         <v>44</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
@@ -3385,19 +3395,19 @@
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>22</v>
+        <v>153</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1" t="s">
@@ -3410,10 +3420,14 @@
         <v>26</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="L43" s="4" t="s">
+        <v>298</v>
+      </c>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
@@ -3431,23 +3445,23 @@
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>301</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>303</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>25</v>
@@ -3477,23 +3491,23 @@
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>305</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>307</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>25</v>
@@ -3523,23 +3537,23 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>309</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>311</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1" t="s">
-        <v>313</v>
+        <v>38</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>25</v>
@@ -3569,23 +3583,23 @@
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1" t="s">
-        <v>33</v>
+        <v>315</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>25</v>
@@ -3615,23 +3629,23 @@
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>318</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>320</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>25</v>
@@ -3640,14 +3654,10 @@
         <v>26</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K48" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="L48" s="4" t="s">
-        <v>323</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
       <c r="M48" s="3"/>
       <c r="N48" s="3"/>
       <c r="O48" s="3"/>
@@ -3665,19 +3675,19 @@
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
@@ -3690,10 +3700,14 @@
         <v>26</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="L49" s="4" t="s">
+        <v>325</v>
+      </c>
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
       <c r="O49" s="3"/>
@@ -3711,23 +3725,23 @@
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>330</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>25</v>
@@ -3757,23 +3771,23 @@
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="D51" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>333</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>25</v>
@@ -3782,14 +3796,10 @@
         <v>26</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K51" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="L51" s="4" t="s">
-        <v>337</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
@@ -3807,23 +3817,23 @@
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>25</v>
@@ -3832,10 +3842,14 @@
         <v>26</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="L52" s="4" t="s">
+        <v>339</v>
+      </c>
       <c r="M52" s="3"/>
       <c r="N52" s="3"/>
       <c r="O52" s="3"/>
@@ -3851,25 +3865,25 @@
       <c r="Y52" s="3"/>
       <c r="Z52" s="3"/>
     </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="D53" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>343</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>346</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="H53" s="2" t="s">
         <v>25</v>
@@ -3878,14 +3892,10 @@
         <v>26</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K53" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="L53" s="4" t="s">
-        <v>348</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
       <c r="M53" s="3"/>
       <c r="N53" s="3"/>
       <c r="O53" s="3"/>
@@ -3901,21 +3911,21 @@
       <c r="Y53" s="3"/>
       <c r="Z53" s="3"/>
     </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1" t="s">
@@ -3931,10 +3941,10 @@
         <v>44</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="M54" s="3"/>
       <c r="N54" s="3"/>
@@ -3953,23 +3963,23 @@
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>25</v>
@@ -3981,10 +3991,10 @@
         <v>44</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="M55" s="3"/>
       <c r="N55" s="3"/>
@@ -4003,19 +4013,19 @@
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1" t="s">
@@ -4031,10 +4041,10 @@
         <v>44</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="M56" s="3"/>
       <c r="N56" s="3"/>
@@ -4051,7 +4061,56 @@
       <c r="Y56" s="3"/>
       <c r="Z56" s="3"/>
     </row>
-    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="L57" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="M57" s="3"/>
+      <c r="N57" s="3"/>
+      <c r="O57" s="3"/>
+      <c r="P57" s="3"/>
+      <c r="Q57" s="3"/>
+      <c r="R57" s="3"/>
+      <c r="S57" s="3"/>
+      <c r="T57" s="3"/>
+      <c r="U57" s="3"/>
+      <c r="V57" s="3"/>
+      <c r="W57" s="3"/>
+      <c r="X57" s="3"/>
+      <c r="Y57" s="3"/>
+      <c r="Z57" s="3"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L5" r:id="rId1" display="https://uk.farnell.com/-/-/-/dp/1758993"/>
@@ -4087,16 +4146,17 @@
     <hyperlink ref="L36" r:id="rId31" display="https://www.mouser.co.uk/ProductDetail/Silicon-Labs/SI8602AC-B-IS?qs=j6MGy4L9yX00K7b%252BnoTSPA%3D%3D"/>
     <hyperlink ref="L37" r:id="rId32" display="https://www.mouser.co.uk/ProductDetail/ON-Semiconductor/STF202-22T1G?qs=%2Fha2pyFadujRFaXPnV9RsTetlaFPPaXSz4EERle60zyiot5T0fRtTg%3D%3D"/>
     <hyperlink ref="L38" r:id="rId33" display="https://uk.farnell.com/-/-/-/dp/2333160"/>
-    <hyperlink ref="L39" r:id="rId34" display="https://uk.farnell.com/-/-/-/dp/2217974"/>
-    <hyperlink ref="L40" r:id="rId35" display="https://uk.farnell.com/-/-/-/dp/1318243"/>
-    <hyperlink ref="L41" r:id="rId36" display="https://uk.farnell.com/-/-/-/dp/1686083"/>
-    <hyperlink ref="L42" r:id="rId37" display="https://uk.farnell.com/-/-/-/dp/1081229"/>
-    <hyperlink ref="L48" r:id="rId38" display="https://uk.farnell.com/-/-/-/dp/2072829"/>
-    <hyperlink ref="L51" r:id="rId39" display="https://uk.farnell.com/-/-/-/dp/1621964"/>
-    <hyperlink ref="L53" r:id="rId40" display="https://uk.farnell.com/-/-/-/dp/3228722"/>
-    <hyperlink ref="L54" r:id="rId41" display="https://uk.farnell.com/-/-/-/dp/1770150"/>
-    <hyperlink ref="L55" r:id="rId42" display="https://uk.farnell.com/-/-/-/dp/1555987"/>
-    <hyperlink ref="L56" r:id="rId43" display="https://uk.farnell.com/-/-/-/dp/1611803"/>
+    <hyperlink ref="L39" r:id="rId34" display="https://www.mouser.co.uk/ProductDetail/STMicroelectronics/STM32F103C6U6A?qs=%2Fha2pyFaduhWlUF2EGqvyLw8AQJjPxdFr9%2FgAGUmVdrlf0EAElETsQ%3D%3D"/>
+    <hyperlink ref="L40" r:id="rId35" display="https://uk.farnell.com/-/-/-/dp/2217974"/>
+    <hyperlink ref="L41" r:id="rId36" display="https://uk.farnell.com/-/-/-/dp/1318243"/>
+    <hyperlink ref="L42" r:id="rId37" display="https://uk.farnell.com/-/-/-/dp/1686083"/>
+    <hyperlink ref="L43" r:id="rId38" display="https://uk.farnell.com/-/-/-/dp/1081229"/>
+    <hyperlink ref="L49" r:id="rId39" display="https://uk.farnell.com/-/-/-/dp/2072829"/>
+    <hyperlink ref="L52" r:id="rId40" display="https://uk.farnell.com/-/-/-/dp/1621964"/>
+    <hyperlink ref="L54" r:id="rId41" display="https://uk.farnell.com/-/-/-/dp/3228722"/>
+    <hyperlink ref="L55" r:id="rId42" display="https://uk.farnell.com/-/-/-/dp/1770150"/>
+    <hyperlink ref="L56" r:id="rId43" display="https://uk.farnell.com/-/-/-/dp/1555987"/>
+    <hyperlink ref="L57" r:id="rId44" display="https://uk.farnell.com/-/-/-/dp/1611803"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Change F1 to better part suggestion
</commit_message>
<xml_diff>
--- a/quote-pack/servo/servo-bom.xlsx
+++ b/quote-pack/servo/servo-bom.xlsx
@@ -661,10 +661,10 @@
     <t xml:space="preserve">200mA 30V resettable fuse</t>
   </si>
   <si>
-    <t xml:space="preserve">3237597</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://uk.farnell.com/-/-/-/dp/3237597</t>
+    <t xml:space="preserve">1206716</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://uk.farnell.com/-/-/-/dp/1206716</t>
   </si>
   <si>
     <t xml:space="preserve">U6</t>
@@ -1267,8 +1267,8 @@
   </sheetPr>
   <dimension ref="A1:Z57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K40" activeCellId="0" sqref="K40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L30" activeCellId="0" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1278,7 +1278,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.39"/>
@@ -4137,7 +4137,7 @@
     <hyperlink ref="L27" r:id="rId22" display="https://uk.farnell.com/-/-/-/dp/1463451"/>
     <hyperlink ref="L28" r:id="rId23" display="https://uk.farnell.com/-/-/-/dp/2053836"/>
     <hyperlink ref="L29" r:id="rId24" display="https://uk.farnell.com/-/-/-/dp/2400368"/>
-    <hyperlink ref="L30" r:id="rId25" display="https://uk.farnell.com/-/-/-/dp/3237597"/>
+    <hyperlink ref="L30" r:id="rId25" display="https://uk.farnell.com/-/-/-/dp/1206716"/>
     <hyperlink ref="L31" r:id="rId26" display="https://uk.farnell.com/-/-/-/dp/3118164"/>
     <hyperlink ref="L32" r:id="rId27" display="https://uk.farnell.com/-/-/-/dp/1439380"/>
     <hyperlink ref="L33" r:id="rId28" display="https://uk.farnell.com/-/-/-/dp/1851953"/>

</xml_diff>